<commit_message>
Last framework backup - @NGC Mumbai
</commit_message>
<xml_diff>
--- a/TestData/CE automation.xlsx
+++ b/TestData/CE automation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shailendra.rajawat\git\iotronApex5\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F99A61B-A4F3-44A1-95C1-6E9D1977CE24}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491F8329-AC94-40F3-BF34-8CD966BE769C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9772,7 +9772,9 @@
   </sheetPr>
   <dimension ref="A1:P1503"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>